<commit_message>
i am a wonder
</commit_message>
<xml_diff>
--- a/dir/New Microsoft Excel Worksheet.xlsx
+++ b/dir/New Microsoft Excel Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\utube WD learning\git things\dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A375A9A6-8B1B-426B-9B9C-1C8D8D5C464C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E2E21E-9F2A-4AF5-BC1E-ECD91F85FD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>dsjljlsdjsljkl</t>
-  </si>
-  <si>
     <t>sdlkajljs</t>
   </si>
   <si>
     <t>djalsjflkjfalskj</t>
+  </si>
+  <si>
+    <t>heheheheh</t>
   </si>
 </sst>
 </file>
@@ -353,25 +353,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>